<commit_message>
SLD-020 changed results folder structure, fixed error handling
</commit_message>
<xml_diff>
--- a/src/main/resources/IndPlanExample.xlsx
+++ b/src/main/resources/IndPlanExample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SLDOCS2023\!data\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDEA\Idea Projects\sldocs\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1A3E90-EAB8-4A55-BC1B-A4F16F90A7B5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="926" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="926" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ТИТУЛ" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">РОЗПОДІЛ!$A$1:$E$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ТИТУЛ!$A$1:$G$40</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -687,7 +688,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* \-??_р_._-;_-@_-"/>
   </numFmts>
@@ -2213,6 +2214,38 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2229,42 +2262,47 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2283,39 +2321,84 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -2328,78 +2411,6 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2436,38 +2447,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2496,23 +2477,43 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1"/>
-    <cellStyle name="Обычный 3" xfId="2"/>
-    <cellStyle name="Обычный 4" xfId="3"/>
-    <cellStyle name="Финансовый 2" xfId="4"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Обычный 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Финансовый 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -2554,9 +2555,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2594,7 +2595,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2629,6 +2630,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2664,9 +2682,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2839,7 +2874,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -2849,33 +2884,33 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
     <col min="5" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="12.33203125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.44140625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="12.28515625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" style="29" customWidth="1"/>
     <col min="13" max="13" width="76" style="29" customWidth="1"/>
-    <col min="14" max="23" width="18.44140625" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.109375" style="1"/>
+    <col min="14" max="23" width="18.42578125" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="54.75" customHeight="1">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
       <c r="H1" s="6"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -2930,23 +2965,23 @@
       <c r="H8" s="13"/>
       <c r="I8" s="12"/>
       <c r="K8" s="13"/>
-      <c r="L8" s="157"/>
-      <c r="M8" s="158"/>
-    </row>
-    <row r="9" spans="1:14" ht="44.4" customHeight="1">
-      <c r="A9" s="244" t="s">
+      <c r="L8" s="160"/>
+      <c r="M8" s="159"/>
+    </row>
+    <row r="9" spans="1:14" ht="44.45" customHeight="1">
+      <c r="A9" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="242" t="s">
+      <c r="B9" s="167" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="242"/>
-      <c r="D9" s="242"/>
-      <c r="E9" s="242"/>
-      <c r="F9" s="242"/>
+      <c r="C9" s="167"/>
+      <c r="D9" s="167"/>
+      <c r="E9" s="167"/>
+      <c r="F9" s="167"/>
       <c r="G9" s="22"/>
-      <c r="L9" s="157"/>
-      <c r="M9" s="158"/>
+      <c r="L9" s="160"/>
+      <c r="M9" s="159"/>
       <c r="N9" s="14"/>
     </row>
     <row r="10" spans="1:14" ht="5.25" customHeight="1">
@@ -2961,7 +2996,7 @@
       <c r="N10" s="14"/>
     </row>
     <row r="11" spans="1:14" ht="6.75" customHeight="1">
-      <c r="A11" s="243" t="s">
+      <c r="A11" s="166" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="24"/>
@@ -2974,22 +3009,22 @@
       <c r="N11" s="14"/>
     </row>
     <row r="12" spans="1:14" ht="42.75" customHeight="1">
-      <c r="A12" s="243"/>
-      <c r="B12" s="156" t="s">
+      <c r="A12" s="166"/>
+      <c r="B12" s="168" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="156"/>
-      <c r="D12" s="156"/>
-      <c r="E12" s="156"/>
-      <c r="F12" s="156"/>
+      <c r="C12" s="168"/>
+      <c r="D12" s="168"/>
+      <c r="E12" s="168"/>
+      <c r="F12" s="168"/>
       <c r="G12" s="21"/>
-      <c r="L12" s="159"/>
-      <c r="M12" s="158"/>
+      <c r="L12" s="158"/>
+      <c r="M12" s="159"/>
       <c r="N12" s="14"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="L13" s="159"/>
-      <c r="M13" s="158"/>
+      <c r="L13" s="158"/>
+      <c r="M13" s="159"/>
       <c r="N13" s="14"/>
     </row>
     <row r="14" spans="1:14">
@@ -3012,16 +3047,16 @@
       <c r="M18" s="28"/>
       <c r="N18" s="14"/>
     </row>
-    <row r="19" spans="1:14" s="9" customFormat="1" ht="30.6">
-      <c r="A19" s="153" t="s">
+    <row r="19" spans="1:14" s="9" customFormat="1" ht="30.75">
+      <c r="A19" s="163" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="153"/>
-      <c r="C19" s="153"/>
-      <c r="D19" s="153"/>
-      <c r="E19" s="153"/>
-      <c r="F19" s="153"/>
-      <c r="G19" s="153"/>
+      <c r="B19" s="163"/>
+      <c r="C19" s="163"/>
+      <c r="D19" s="163"/>
+      <c r="E19" s="163"/>
+      <c r="F19" s="163"/>
+      <c r="G19" s="163"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
       <c r="K19" s="17"/>
@@ -3030,15 +3065,15 @@
       <c r="N19" s="14"/>
     </row>
     <row r="20" spans="1:14" s="10" customFormat="1" ht="18" customHeight="1">
-      <c r="A20" s="154" t="s">
+      <c r="A20" s="164" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="154"/>
-      <c r="C20" s="154"/>
-      <c r="D20" s="154"/>
-      <c r="E20" s="154"/>
-      <c r="F20" s="154"/>
-      <c r="G20" s="154"/>
+      <c r="B20" s="164"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="164"/>
+      <c r="F20" s="164"/>
+      <c r="G20" s="164"/>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
       <c r="K20" s="18"/>
@@ -3079,32 +3114,32 @@
       <c r="M23" s="28"/>
       <c r="N23" s="14"/>
     </row>
-    <row r="24" spans="1:14" ht="24.6">
-      <c r="A24" s="155" t="s">
+    <row r="24" spans="1:14" ht="25.5">
+      <c r="A24" s="165" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="155"/>
-      <c r="C24" s="155"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="155"/>
-      <c r="F24" s="155"/>
-      <c r="G24" s="155"/>
-      <c r="L24" s="159"/>
-      <c r="M24" s="158"/>
+      <c r="B24" s="165"/>
+      <c r="C24" s="165"/>
+      <c r="D24" s="165"/>
+      <c r="E24" s="165"/>
+      <c r="F24" s="165"/>
+      <c r="G24" s="165"/>
+      <c r="L24" s="158"/>
+      <c r="M24" s="159"/>
       <c r="N24" s="14"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="151" t="s">
+      <c r="A25" s="161" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="151"/>
-      <c r="C25" s="151"/>
-      <c r="D25" s="151"/>
-      <c r="E25" s="151"/>
-      <c r="F25" s="151"/>
-      <c r="G25" s="151"/>
-      <c r="L25" s="159"/>
-      <c r="M25" s="158"/>
+      <c r="B25" s="161"/>
+      <c r="C25" s="161"/>
+      <c r="D25" s="161"/>
+      <c r="E25" s="161"/>
+      <c r="F25" s="161"/>
+      <c r="G25" s="161"/>
+      <c r="L25" s="158"/>
+      <c r="M25" s="159"/>
       <c r="N25" s="14"/>
     </row>
     <row r="26" spans="1:14">
@@ -3193,10 +3228,10 @@
       <c r="E33" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="162" t="s">
+      <c r="F33" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="G33" s="163"/>
+      <c r="G33" s="155"/>
       <c r="M33" s="28"/>
       <c r="N33" s="14"/>
     </row>
@@ -3216,18 +3251,18 @@
       <c r="E34" s="67">
         <v>1.5</v>
       </c>
-      <c r="F34" s="164" t="s">
+      <c r="F34" s="156" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="165"/>
-      <c r="L34" s="159"/>
-      <c r="M34" s="158"/>
+      <c r="G34" s="157"/>
+      <c r="L34" s="158"/>
+      <c r="M34" s="159"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="L35" s="159"/>
-      <c r="M35" s="158"/>
-    </row>
-    <row r="36" spans="1:14" ht="18">
+      <c r="L35" s="158"/>
+      <c r="M35" s="159"/>
+    </row>
+    <row r="36" spans="1:14" ht="18.75">
       <c r="B36" s="105" t="s">
         <v>14</v>
       </c>
@@ -3236,30 +3271,30 @@
       </c>
       <c r="D36" s="125"/>
       <c r="E36" s="125"/>
-      <c r="M36" s="161"/>
-    </row>
-    <row r="37" spans="1:14" ht="18">
+      <c r="M36" s="153"/>
+    </row>
+    <row r="37" spans="1:14" ht="18.75">
       <c r="B37" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="160" t="s">
+      <c r="C37" s="152" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="160"/>
-      <c r="E37" s="160"/>
-      <c r="M37" s="161"/>
-    </row>
-    <row r="38" spans="1:14" ht="18">
+      <c r="D37" s="152"/>
+      <c r="E37" s="152"/>
+      <c r="M37" s="153"/>
+    </row>
+    <row r="38" spans="1:14" ht="18.75">
       <c r="B38" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="160" t="s">
+      <c r="C38" s="152" t="s">
         <v>95</v>
       </c>
-      <c r="D38" s="160"/>
-      <c r="E38" s="160"/>
-    </row>
-    <row r="39" spans="1:14" ht="21">
+      <c r="D38" s="152"/>
+      <c r="E38" s="152"/>
+    </row>
+    <row r="39" spans="1:14" ht="20.25">
       <c r="B39" s="105" t="s">
         <v>16</v>
       </c>
@@ -3281,19 +3316,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A19:G19"/>
@@ -3302,10 +3324,23 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="M34:M35"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$I$2:$I$8</formula1>
     </dataValidation>
   </dataValidations>
@@ -3317,64 +3352,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="11"/>
+    <col min="1" max="1" width="15.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
     </row>
     <row r="2" spans="1:5" ht="58.5" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="169"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1"/>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
     </row>
     <row r="4" spans="1:5" ht="66" customHeight="1">
-      <c r="A4" s="166"/>
-      <c r="B4" s="166"/>
-      <c r="C4" s="166"/>
-      <c r="D4" s="166"/>
-      <c r="E4" s="166"/>
+      <c r="A4" s="169"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="166"/>
-      <c r="B5" s="166"/>
-      <c r="C5" s="166"/>
-      <c r="D5" s="166"/>
-      <c r="E5" s="166"/>
+      <c r="A5" s="169"/>
+      <c r="B5" s="169"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="166"/>
-      <c r="B6" s="166"/>
-      <c r="C6" s="166"/>
-      <c r="D6" s="166"/>
-      <c r="E6" s="166"/>
+      <c r="A6" s="169"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
@@ -3391,27 +3426,27 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="166"/>
-      <c r="B9" s="166"/>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="166"/>
+      <c r="A9" s="169"/>
+      <c r="B9" s="169"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="166"/>
-      <c r="B10" s="166"/>
-      <c r="C10" s="166"/>
-      <c r="D10" s="166"/>
-      <c r="E10" s="166"/>
+      <c r="A10" s="169"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="169"/>
+      <c r="D10" s="169"/>
+      <c r="E10" s="169"/>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A11" s="167" t="s">
+      <c r="A11" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="166"/>
-      <c r="C11" s="166"/>
-      <c r="D11" s="166"/>
-      <c r="E11" s="166"/>
+      <c r="B11" s="169"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="169"/>
+      <c r="E11" s="169"/>
     </row>
     <row r="12" spans="1:5" ht="21" customHeight="1" thickBot="1">
       <c r="A12" s="121"/>
@@ -3421,20 +3456,20 @@
       <c r="E12" s="121"/>
     </row>
     <row r="13" spans="1:5" ht="30.75" customHeight="1">
-      <c r="A13" s="168" t="s">
+      <c r="A13" s="180" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="169"/>
-      <c r="C13" s="169"/>
-      <c r="D13" s="169"/>
-      <c r="E13" s="170"/>
+      <c r="B13" s="181"/>
+      <c r="C13" s="181"/>
+      <c r="D13" s="181"/>
+      <c r="E13" s="182"/>
     </row>
     <row r="14" spans="1:5" ht="26.25" customHeight="1">
-      <c r="A14" s="171" t="s">
+      <c r="A14" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="171"/>
-      <c r="C14" s="172"/>
+      <c r="B14" s="183"/>
+      <c r="C14" s="184"/>
       <c r="D14" s="122" t="s">
         <v>21</v>
       </c>
@@ -3443,47 +3478,47 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1">
-      <c r="A15" s="174" t="s">
+      <c r="A15" s="171" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="174"/>
-      <c r="C15" s="174"/>
+      <c r="B15" s="171"/>
+      <c r="C15" s="171"/>
       <c r="D15" s="146"/>
       <c r="E15" s="146"/>
     </row>
     <row r="16" spans="1:5" ht="33" customHeight="1">
-      <c r="A16" s="175" t="s">
+      <c r="A16" s="172" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="176"/>
-      <c r="C16" s="176"/>
+      <c r="B16" s="173"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="146"/>
       <c r="E16" s="146"/>
     </row>
     <row r="17" spans="1:5" ht="27.75" customHeight="1">
-      <c r="A17" s="177" t="s">
+      <c r="A17" s="174" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="174"/>
-      <c r="C17" s="174"/>
+      <c r="B17" s="171"/>
+      <c r="C17" s="171"/>
       <c r="D17" s="146"/>
       <c r="E17" s="146"/>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" thickBot="1">
-      <c r="A18" s="178" t="s">
+      <c r="A18" s="175" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="178"/>
-      <c r="C18" s="178"/>
+      <c r="B18" s="175"/>
+      <c r="C18" s="175"/>
       <c r="D18" s="145"/>
       <c r="E18" s="145"/>
     </row>
     <row r="19" spans="1:5" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A19" s="179" t="s">
+      <c r="A19" s="176" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="180"/>
-      <c r="C19" s="181"/>
+      <c r="B19" s="177"/>
+      <c r="C19" s="178"/>
       <c r="D19" s="124">
         <f>SUM(D15:D18)</f>
         <v>0</v>
@@ -3508,20 +3543,20 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="54" customHeight="1">
-      <c r="A22" s="166"/>
-      <c r="B22" s="166"/>
-      <c r="C22" s="166"/>
-      <c r="D22" s="166"/>
-      <c r="E22" s="166"/>
+      <c r="A22" s="169"/>
+      <c r="B22" s="169"/>
+      <c r="C22" s="169"/>
+      <c r="D22" s="169"/>
+      <c r="E22" s="169"/>
     </row>
     <row r="23" spans="1:5" ht="17.25" customHeight="1">
-      <c r="A23" s="173" t="s">
+      <c r="A23" s="170" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="173"/>
-      <c r="C23" s="173"/>
-      <c r="D23" s="173"/>
-      <c r="E23" s="173"/>
+      <c r="B23" s="170"/>
+      <c r="C23" s="170"/>
+      <c r="D23" s="170"/>
+      <c r="E23" s="170"/>
     </row>
     <row r="24" spans="1:5" ht="36" customHeight="1">
       <c r="A24" s="1"/>
@@ -3531,13 +3566,13 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1">
-      <c r="A25" s="173" t="s">
+      <c r="A25" s="170" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="173"/>
-      <c r="C25" s="173"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="173"/>
+      <c r="B25" s="170"/>
+      <c r="C25" s="170"/>
+      <c r="D25" s="170"/>
+      <c r="E25" s="170"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1"/>
@@ -3548,6 +3583,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C1:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:C14"/>
     <mergeCell ref="A22:E22"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="A25:E25"/>
@@ -3556,16 +3601,6 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="C1:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3573,71 +3608,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BA70"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="87" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="R21" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="87" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BA67" sqref="BA67"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" style="34" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" style="33" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.6640625" style="100" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" style="14" customWidth="1"/>
-    <col min="12" max="12" width="5.109375" style="33" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="5.109375" style="33" customWidth="1"/>
-    <col min="15" max="15" width="5.109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="5.109375" style="33" customWidth="1"/>
-    <col min="19" max="19" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="4.109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="5.88671875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="4.33203125" style="1" customWidth="1"/>
-    <col min="24" max="25" width="5.109375" style="33" customWidth="1"/>
-    <col min="26" max="27" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.88671875" style="33" customWidth="1"/>
-    <col min="29" max="29" width="5.109375" style="33" customWidth="1"/>
-    <col min="30" max="31" width="5.109375" style="1" customWidth="1"/>
-    <col min="32" max="32" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.6640625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="4.44140625" style="33" customWidth="1"/>
-    <col min="35" max="35" width="5.109375" style="33" customWidth="1"/>
-    <col min="36" max="36" width="3.6640625" style="33" customWidth="1"/>
-    <col min="37" max="37" width="4.5546875" style="33" customWidth="1"/>
-    <col min="38" max="39" width="5.109375" style="1" customWidth="1"/>
-    <col min="40" max="41" width="4.6640625" style="1" customWidth="1"/>
-    <col min="42" max="42" width="4.33203125" style="14" customWidth="1"/>
-    <col min="43" max="43" width="4.109375" style="14" customWidth="1"/>
-    <col min="44" max="45" width="4.44140625" style="1" customWidth="1"/>
-    <col min="46" max="46" width="3.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="34" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="33" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" style="100" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" style="14" customWidth="1"/>
+    <col min="12" max="12" width="5.140625" style="33" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="5.140625" style="33" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="5.140625" style="33" customWidth="1"/>
+    <col min="19" max="19" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="4.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="5.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="4.28515625" style="1" customWidth="1"/>
+    <col min="24" max="25" width="5.140625" style="33" customWidth="1"/>
+    <col min="26" max="27" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.85546875" style="33" customWidth="1"/>
+    <col min="29" max="29" width="5.140625" style="33" customWidth="1"/>
+    <col min="30" max="31" width="5.140625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.7109375" style="1" customWidth="1"/>
+    <col min="34" max="34" width="4.42578125" style="33" customWidth="1"/>
+    <col min="35" max="35" width="5.140625" style="33" customWidth="1"/>
+    <col min="36" max="36" width="3.7109375" style="33" customWidth="1"/>
+    <col min="37" max="37" width="4.5703125" style="33" customWidth="1"/>
+    <col min="38" max="39" width="5.140625" style="1" customWidth="1"/>
+    <col min="40" max="41" width="4.7109375" style="1" customWidth="1"/>
+    <col min="42" max="42" width="4.28515625" style="14" customWidth="1"/>
+    <col min="43" max="43" width="4.140625" style="14" customWidth="1"/>
+    <col min="44" max="45" width="4.42578125" style="1" customWidth="1"/>
+    <col min="46" max="46" width="3.85546875" style="1" customWidth="1"/>
     <col min="47" max="47" width="4" style="1" customWidth="1"/>
-    <col min="48" max="49" width="4.5546875" style="1" customWidth="1"/>
-    <col min="50" max="51" width="5.6640625" style="2" customWidth="1"/>
+    <col min="48" max="49" width="4.5703125" style="1" customWidth="1"/>
+    <col min="50" max="51" width="5.7109375" style="2" customWidth="1"/>
     <col min="52" max="52" width="11" style="1" customWidth="1"/>
-    <col min="53" max="53" width="8.5546875" style="1" customWidth="1"/>
-    <col min="54" max="54" width="11.5546875" style="1" customWidth="1"/>
-    <col min="55" max="16384" width="9.109375" style="1"/>
+    <col min="53" max="53" width="8.5703125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="11.5703125" style="1" customWidth="1"/>
+    <col min="55" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="101" customFormat="1" ht="16.2" thickBot="1">
+    <row r="1" spans="1:51" s="101" customFormat="1" ht="16.5" thickBot="1">
       <c r="A1" s="112" t="s">
         <v>24</v>
       </c>
@@ -3693,177 +3728,177 @@
       <c r="AY1" s="110"/>
     </row>
     <row r="2" spans="1:51" s="110" customFormat="1" ht="36" customHeight="1">
-      <c r="A2" s="188" t="s">
+      <c r="A2" s="185" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="188" t="s">
+      <c r="B2" s="185" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="209" t="s">
+      <c r="C2" s="199" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="209" t="s">
+      <c r="D2" s="199" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="186" t="s">
+      <c r="E2" s="213" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="188" t="s">
+      <c r="F2" s="185" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="188" t="s">
+      <c r="G2" s="185" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="191" t="s">
+      <c r="H2" s="192" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="192"/>
-      <c r="J2" s="191" t="s">
+      <c r="I2" s="196"/>
+      <c r="J2" s="192" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="192"/>
-      <c r="L2" s="191" t="s">
+      <c r="K2" s="196"/>
+      <c r="L2" s="192" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="192"/>
-      <c r="N2" s="191" t="s">
+      <c r="M2" s="196"/>
+      <c r="N2" s="192" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="192"/>
-      <c r="P2" s="191" t="s">
+      <c r="O2" s="196"/>
+      <c r="P2" s="192" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="183"/>
-      <c r="R2" s="191" t="s">
+      <c r="Q2" s="193"/>
+      <c r="R2" s="192" t="s">
         <v>79</v>
       </c>
-      <c r="S2" s="183"/>
-      <c r="T2" s="197" t="s">
+      <c r="S2" s="193"/>
+      <c r="T2" s="188" t="s">
         <v>80</v>
       </c>
-      <c r="U2" s="198"/>
-      <c r="V2" s="191" t="s">
+      <c r="U2" s="189"/>
+      <c r="V2" s="192" t="s">
         <v>81</v>
       </c>
-      <c r="W2" s="192"/>
-      <c r="X2" s="197" t="s">
+      <c r="W2" s="196"/>
+      <c r="X2" s="188" t="s">
         <v>82</v>
       </c>
-      <c r="Y2" s="198"/>
-      <c r="Z2" s="197" t="s">
+      <c r="Y2" s="189"/>
+      <c r="Z2" s="188" t="s">
         <v>83</v>
       </c>
-      <c r="AA2" s="198"/>
-      <c r="AB2" s="197" t="s">
+      <c r="AA2" s="189"/>
+      <c r="AB2" s="188" t="s">
         <v>84</v>
       </c>
-      <c r="AC2" s="198"/>
-      <c r="AD2" s="201" t="s">
+      <c r="AC2" s="189"/>
+      <c r="AD2" s="206" t="s">
         <v>85</v>
       </c>
-      <c r="AE2" s="202"/>
-      <c r="AF2" s="197" t="s">
+      <c r="AE2" s="207"/>
+      <c r="AF2" s="188" t="s">
         <v>86</v>
       </c>
-      <c r="AG2" s="198"/>
-      <c r="AH2" s="197" t="s">
+      <c r="AG2" s="189"/>
+      <c r="AH2" s="188" t="s">
         <v>87</v>
       </c>
-      <c r="AI2" s="198"/>
-      <c r="AJ2" s="197" t="s">
+      <c r="AI2" s="189"/>
+      <c r="AJ2" s="188" t="s">
         <v>88</v>
       </c>
-      <c r="AK2" s="198"/>
-      <c r="AL2" s="197" t="s">
+      <c r="AK2" s="189"/>
+      <c r="AL2" s="188" t="s">
         <v>34</v>
       </c>
-      <c r="AM2" s="198"/>
-      <c r="AN2" s="197" t="s">
+      <c r="AM2" s="189"/>
+      <c r="AN2" s="188" t="s">
         <v>35</v>
       </c>
-      <c r="AO2" s="198"/>
-      <c r="AP2" s="197" t="s">
+      <c r="AO2" s="189"/>
+      <c r="AP2" s="188" t="s">
         <v>36</v>
       </c>
-      <c r="AQ2" s="198"/>
-      <c r="AR2" s="201" t="s">
+      <c r="AQ2" s="189"/>
+      <c r="AR2" s="206" t="s">
         <v>37</v>
       </c>
-      <c r="AS2" s="202"/>
-      <c r="AT2" s="191" t="s">
+      <c r="AS2" s="207"/>
+      <c r="AT2" s="192" t="s">
         <v>38</v>
       </c>
-      <c r="AU2" s="205"/>
-      <c r="AV2" s="207" t="s">
+      <c r="AU2" s="203"/>
+      <c r="AV2" s="205" t="s">
         <v>39</v>
       </c>
-      <c r="AW2" s="198"/>
-      <c r="AX2" s="182" t="s">
+      <c r="AW2" s="189"/>
+      <c r="AX2" s="210" t="s">
         <v>40</v>
       </c>
-      <c r="AY2" s="183"/>
+      <c r="AY2" s="193"/>
     </row>
     <row r="3" spans="1:51" s="110" customFormat="1" ht="119.25" customHeight="1" thickBot="1">
-      <c r="A3" s="189"/>
-      <c r="B3" s="189"/>
-      <c r="C3" s="210"/>
-      <c r="D3" s="210"/>
-      <c r="E3" s="187"/>
-      <c r="F3" s="189"/>
-      <c r="G3" s="189"/>
-      <c r="H3" s="193"/>
-      <c r="I3" s="194"/>
-      <c r="J3" s="193"/>
-      <c r="K3" s="194"/>
-      <c r="L3" s="193"/>
-      <c r="M3" s="194"/>
-      <c r="N3" s="193"/>
-      <c r="O3" s="194"/>
-      <c r="P3" s="195"/>
-      <c r="Q3" s="196"/>
-      <c r="R3" s="195"/>
-      <c r="S3" s="196"/>
-      <c r="T3" s="208"/>
-      <c r="U3" s="200"/>
-      <c r="V3" s="193"/>
-      <c r="W3" s="194"/>
-      <c r="X3" s="199"/>
-      <c r="Y3" s="200"/>
-      <c r="Z3" s="199"/>
-      <c r="AA3" s="200"/>
-      <c r="AB3" s="199"/>
-      <c r="AC3" s="200"/>
-      <c r="AD3" s="203"/>
-      <c r="AE3" s="204"/>
-      <c r="AF3" s="199"/>
-      <c r="AG3" s="200"/>
-      <c r="AH3" s="199"/>
-      <c r="AI3" s="200"/>
-      <c r="AJ3" s="199"/>
-      <c r="AK3" s="200"/>
-      <c r="AL3" s="199"/>
-      <c r="AM3" s="200"/>
-      <c r="AN3" s="199"/>
-      <c r="AO3" s="200"/>
-      <c r="AP3" s="199"/>
-      <c r="AQ3" s="200"/>
-      <c r="AR3" s="203"/>
-      <c r="AS3" s="204"/>
-      <c r="AT3" s="199"/>
-      <c r="AU3" s="206"/>
-      <c r="AV3" s="206"/>
-      <c r="AW3" s="200"/>
-      <c r="AX3" s="184"/>
-      <c r="AY3" s="185"/>
-    </row>
-    <row r="4" spans="1:51" s="101" customFormat="1" ht="16.2" thickBot="1">
-      <c r="A4" s="190"/>
-      <c r="B4" s="190"/>
-      <c r="C4" s="211"/>
-      <c r="D4" s="211"/>
-      <c r="E4" s="187"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="190"/>
+      <c r="A3" s="186"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="214"/>
+      <c r="F3" s="186"/>
+      <c r="G3" s="186"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="198"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="198"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="198"/>
+      <c r="N3" s="197"/>
+      <c r="O3" s="198"/>
+      <c r="P3" s="194"/>
+      <c r="Q3" s="195"/>
+      <c r="R3" s="194"/>
+      <c r="S3" s="195"/>
+      <c r="T3" s="190"/>
+      <c r="U3" s="191"/>
+      <c r="V3" s="197"/>
+      <c r="W3" s="198"/>
+      <c r="X3" s="202"/>
+      <c r="Y3" s="191"/>
+      <c r="Z3" s="202"/>
+      <c r="AA3" s="191"/>
+      <c r="AB3" s="202"/>
+      <c r="AC3" s="191"/>
+      <c r="AD3" s="208"/>
+      <c r="AE3" s="209"/>
+      <c r="AF3" s="202"/>
+      <c r="AG3" s="191"/>
+      <c r="AH3" s="202"/>
+      <c r="AI3" s="191"/>
+      <c r="AJ3" s="202"/>
+      <c r="AK3" s="191"/>
+      <c r="AL3" s="202"/>
+      <c r="AM3" s="191"/>
+      <c r="AN3" s="202"/>
+      <c r="AO3" s="191"/>
+      <c r="AP3" s="202"/>
+      <c r="AQ3" s="191"/>
+      <c r="AR3" s="208"/>
+      <c r="AS3" s="209"/>
+      <c r="AT3" s="202"/>
+      <c r="AU3" s="204"/>
+      <c r="AV3" s="204"/>
+      <c r="AW3" s="191"/>
+      <c r="AX3" s="211"/>
+      <c r="AY3" s="212"/>
+    </row>
+    <row r="4" spans="1:51" s="101" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A4" s="187"/>
+      <c r="B4" s="187"/>
+      <c r="C4" s="201"/>
+      <c r="D4" s="201"/>
+      <c r="E4" s="214"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="187"/>
       <c r="H4" s="117" t="s">
         <v>41</v>
       </c>
@@ -3997,7 +4032,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="5" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A5" s="104"/>
       <c r="B5" s="104"/>
       <c r="C5" s="104"/>
@@ -4050,7 +4085,7 @@
       <c r="AX5" s="104"/>
       <c r="AY5" s="104"/>
     </row>
-    <row r="6" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="6" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A6" s="104"/>
       <c r="B6" s="104"/>
       <c r="C6" s="104"/>
@@ -4103,7 +4138,7 @@
       <c r="AX6" s="104"/>
       <c r="AY6" s="104"/>
     </row>
-    <row r="7" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="7" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A7" s="104"/>
       <c r="B7" s="104"/>
       <c r="C7" s="104"/>
@@ -4156,7 +4191,7 @@
       <c r="AX7" s="104"/>
       <c r="AY7" s="104"/>
     </row>
-    <row r="8" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="8" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A8" s="104"/>
       <c r="B8" s="104"/>
       <c r="C8" s="104"/>
@@ -4209,7 +4244,7 @@
       <c r="AX8" s="104"/>
       <c r="AY8" s="104"/>
     </row>
-    <row r="9" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="9" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A9" s="104"/>
       <c r="B9" s="104"/>
       <c r="C9" s="104"/>
@@ -4262,7 +4297,7 @@
       <c r="AX9" s="104"/>
       <c r="AY9" s="104"/>
     </row>
-    <row r="10" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="10" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A10" s="104"/>
       <c r="B10" s="104"/>
       <c r="C10" s="104"/>
@@ -4315,7 +4350,7 @@
       <c r="AX10" s="104"/>
       <c r="AY10" s="104"/>
     </row>
-    <row r="11" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="11" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A11" s="104"/>
       <c r="B11" s="104"/>
       <c r="C11" s="104"/>
@@ -4368,7 +4403,7 @@
       <c r="AX11" s="104"/>
       <c r="AY11" s="104"/>
     </row>
-    <row r="12" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="12" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A12" s="104"/>
       <c r="B12" s="104"/>
       <c r="C12" s="104"/>
@@ -4421,7 +4456,7 @@
       <c r="AX12" s="104"/>
       <c r="AY12" s="104"/>
     </row>
-    <row r="13" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="13" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A13" s="104"/>
       <c r="B13" s="104"/>
       <c r="C13" s="104"/>
@@ -4474,7 +4509,7 @@
       <c r="AX13" s="104"/>
       <c r="AY13" s="104"/>
     </row>
-    <row r="14" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="14" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A14" s="104"/>
       <c r="B14" s="104"/>
       <c r="C14" s="104"/>
@@ -4527,7 +4562,7 @@
       <c r="AX14" s="104"/>
       <c r="AY14" s="104"/>
     </row>
-    <row r="15" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="15" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A15" s="104"/>
       <c r="B15" s="104"/>
       <c r="C15" s="104"/>
@@ -5375,7 +5410,7 @@
       <c r="AX30" s="104"/>
       <c r="AY30" s="104"/>
     </row>
-    <row r="31" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="31" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A31" s="104"/>
       <c r="B31" s="104"/>
       <c r="C31" s="104"/>
@@ -5428,7 +5463,7 @@
       <c r="AX31" s="104"/>
       <c r="AY31" s="104"/>
     </row>
-    <row r="32" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="32" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A32" s="104"/>
       <c r="B32" s="104"/>
       <c r="C32" s="104"/>
@@ -5481,7 +5516,7 @@
       <c r="AX32" s="104"/>
       <c r="AY32" s="104"/>
     </row>
-    <row r="33" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="33" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A33" s="104"/>
       <c r="B33" s="104"/>
       <c r="C33" s="104"/>
@@ -5534,7 +5569,7 @@
       <c r="AX33" s="104"/>
       <c r="AY33" s="104"/>
     </row>
-    <row r="34" spans="1:51" s="101" customFormat="1" ht="36.450000000000003" customHeight="1">
+    <row r="34" spans="1:51" s="101" customFormat="1" ht="36.4" customHeight="1">
       <c r="A34" s="104"/>
       <c r="B34" s="104"/>
       <c r="C34" s="104"/>
@@ -5587,7 +5622,7 @@
       <c r="AX34" s="104"/>
       <c r="AY34" s="104"/>
     </row>
-    <row r="35" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="35" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A35" s="104"/>
       <c r="B35" s="104"/>
       <c r="C35" s="104"/>
@@ -5640,7 +5675,7 @@
       <c r="AX35" s="104"/>
       <c r="AY35" s="104"/>
     </row>
-    <row r="36" spans="1:51" s="101" customFormat="1" ht="36.450000000000003" customHeight="1">
+    <row r="36" spans="1:51" s="101" customFormat="1" ht="36.4" customHeight="1">
       <c r="A36" s="104"/>
       <c r="B36" s="104"/>
       <c r="C36" s="104"/>
@@ -5693,7 +5728,7 @@
       <c r="AX36" s="104"/>
       <c r="AY36" s="104"/>
     </row>
-    <row r="37" spans="1:51" s="101" customFormat="1" ht="36.450000000000003" customHeight="1">
+    <row r="37" spans="1:51" s="101" customFormat="1" ht="36.4" customHeight="1">
       <c r="A37" s="104"/>
       <c r="B37" s="104"/>
       <c r="C37" s="104"/>
@@ -5746,7 +5781,7 @@
       <c r="AX37" s="104"/>
       <c r="AY37" s="104"/>
     </row>
-    <row r="38" spans="1:51" s="101" customFormat="1" ht="36.450000000000003" customHeight="1">
+    <row r="38" spans="1:51" s="101" customFormat="1" ht="36.4" customHeight="1">
       <c r="A38" s="104"/>
       <c r="B38" s="104"/>
       <c r="C38" s="104"/>
@@ -5799,7 +5834,7 @@
       <c r="AX38" s="104"/>
       <c r="AY38" s="104"/>
     </row>
-    <row r="39" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="39" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A39" s="104"/>
       <c r="B39" s="104"/>
       <c r="C39" s="104"/>
@@ -5852,7 +5887,7 @@
       <c r="AX39" s="104"/>
       <c r="AY39" s="104"/>
     </row>
-    <row r="40" spans="1:51" s="101" customFormat="1" ht="15.6">
+    <row r="40" spans="1:51" s="101" customFormat="1" ht="15.75">
       <c r="A40" s="104"/>
       <c r="B40" s="104"/>
       <c r="C40" s="104"/>
@@ -6276,7 +6311,7 @@
       <c r="AX47" s="104"/>
       <c r="AY47" s="104"/>
     </row>
-    <row r="48" spans="1:51" s="101" customFormat="1" ht="16.2" hidden="1" customHeight="1" thickBot="1">
+    <row r="48" spans="1:51" s="101" customFormat="1" ht="16.149999999999999" hidden="1" customHeight="1" thickBot="1">
       <c r="A48" s="104"/>
       <c r="B48" s="104"/>
       <c r="C48" s="104"/>
@@ -7283,14 +7318,14 @@
       <c r="AX66" s="104"/>
       <c r="AY66" s="104"/>
     </row>
-    <row r="67" spans="1:53" s="104" customFormat="1" ht="15.6">
+    <row r="67" spans="1:53" s="104" customFormat="1" ht="15.75">
       <c r="BA67" s="104" t="e">
         <f>VLOOKUP(ТИТУЛ!B12,#REF!,2,FALSE)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="68" spans="1:53" s="104" customFormat="1" ht="6" customHeight="1"/>
-    <row r="69" spans="1:53" s="104" customFormat="1" ht="15.6">
+    <row r="69" spans="1:53" s="104" customFormat="1" ht="15.75">
       <c r="BA69" s="104" t="e">
         <f>VLOOKUP(ТИТУЛ!B9,#REF!,3,FALSE)</f>
         <v>#REF!</v>
@@ -7317,19 +7352,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="T2:U3"/>
-    <mergeCell ref="R2:S3"/>
-    <mergeCell ref="H2:I3"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="AN2:AO3"/>
-    <mergeCell ref="AP2:AQ3"/>
-    <mergeCell ref="AT2:AU3"/>
-    <mergeCell ref="AV2:AW3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="AR2:AS3"/>
     <mergeCell ref="AX2:AY3"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:F4"/>
@@ -7346,6 +7368,19 @@
     <mergeCell ref="AH2:AI3"/>
     <mergeCell ref="AJ2:AK3"/>
     <mergeCell ref="AL2:AM3"/>
+    <mergeCell ref="AN2:AO3"/>
+    <mergeCell ref="AP2:AQ3"/>
+    <mergeCell ref="AT2:AU3"/>
+    <mergeCell ref="AV2:AW3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="AR2:AS3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="T2:U3"/>
+    <mergeCell ref="R2:S3"/>
+    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AX62:AY63 H19:H30 H16:L16 M13:M16 N13:N30 O13:O32 N30:AW30 I17:M30 N60:AW60 H65:AY65 H13:I15 K13:L15 R11:S11 W31:AY35 I33 K31:K36 M31:M35 Q31:S31 K38:K40 M40 P12:S30 I36 M37 Q36:S40 R34:S35 U33:U35 Q33:S33 R32:S32 I38:I40 T34:T40 O34:O40 H41:T60 U36:AY60 T13:AY30 X5:AY12 T11:W12">
@@ -7368,7 +7403,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="46" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="47" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="23" max="45" man="1"/>
@@ -7377,7 +7412,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -7387,26 +7422,26 @@
       <selection activeCell="A20" sqref="A20:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="65" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="12.85546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" thickBot="1">
-      <c r="A1" s="212" t="s">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1">
+      <c r="A1" s="215" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-    </row>
-    <row r="2" spans="1:9" ht="78.599999999999994" thickBot="1">
+      <c r="B1" s="215"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+    </row>
+    <row r="2" spans="1:9" ht="79.5" thickBot="1">
       <c r="A2" s="62" t="s">
         <v>44</v>
       </c>
@@ -7429,7 +7464,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" s="40" customFormat="1" ht="18">
+    <row r="3" spans="1:9" s="40" customFormat="1" ht="18.75">
       <c r="A3" s="92"/>
       <c r="B3" s="69"/>
       <c r="C3" s="36"/>
@@ -7440,7 +7475,7 @@
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
     </row>
-    <row r="4" spans="1:9" s="40" customFormat="1" ht="18.600000000000001" thickBot="1">
+    <row r="4" spans="1:9" s="40" customFormat="1" ht="19.5" thickBot="1">
       <c r="A4" s="41"/>
       <c r="B4" s="70"/>
       <c r="C4" s="38"/>
@@ -7451,7 +7486,7 @@
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
     </row>
-    <row r="5" spans="1:9" s="40" customFormat="1" ht="18">
+    <row r="5" spans="1:9" s="40" customFormat="1" ht="18.75">
       <c r="A5" s="92"/>
       <c r="B5" s="70"/>
       <c r="C5" s="38"/>
@@ -7462,7 +7497,7 @@
       <c r="H5" s="39"/>
       <c r="I5" s="39"/>
     </row>
-    <row r="6" spans="1:9" s="40" customFormat="1" ht="18.600000000000001" thickBot="1">
+    <row r="6" spans="1:9" s="40" customFormat="1" ht="19.5" thickBot="1">
       <c r="A6" s="41"/>
       <c r="B6" s="70"/>
       <c r="C6" s="38"/>
@@ -7473,7 +7508,7 @@
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
     </row>
-    <row r="7" spans="1:9" s="40" customFormat="1" ht="18">
+    <row r="7" spans="1:9" s="40" customFormat="1" ht="18.75">
       <c r="A7" s="92"/>
       <c r="B7" s="70"/>
       <c r="C7" s="38"/>
@@ -7484,7 +7519,7 @@
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
     </row>
-    <row r="8" spans="1:9" s="40" customFormat="1" ht="18.600000000000001" thickBot="1">
+    <row r="8" spans="1:9" s="40" customFormat="1" ht="19.5" thickBot="1">
       <c r="A8" s="41"/>
       <c r="B8" s="70"/>
       <c r="C8" s="38"/>
@@ -7495,7 +7530,7 @@
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
     </row>
-    <row r="9" spans="1:9" s="40" customFormat="1" ht="18">
+    <row r="9" spans="1:9" s="40" customFormat="1" ht="18.75">
       <c r="A9" s="92"/>
       <c r="B9" s="80"/>
       <c r="C9" s="38"/>
@@ -7506,7 +7541,7 @@
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
     </row>
-    <row r="10" spans="1:9" s="40" customFormat="1" ht="18.600000000000001" thickBot="1">
+    <row r="10" spans="1:9" s="40" customFormat="1" ht="19.5" thickBot="1">
       <c r="A10" s="41"/>
       <c r="B10" s="93"/>
       <c r="C10" s="38"/>
@@ -7517,7 +7552,7 @@
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
     </row>
-    <row r="11" spans="1:9" s="40" customFormat="1" ht="18">
+    <row r="11" spans="1:9" s="40" customFormat="1" ht="18.75">
       <c r="A11" s="92"/>
       <c r="B11" s="94"/>
       <c r="C11" s="38"/>
@@ -7528,7 +7563,7 @@
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
     </row>
-    <row r="12" spans="1:9" s="40" customFormat="1" ht="18">
+    <row r="12" spans="1:9" s="40" customFormat="1" ht="18.75">
       <c r="A12" s="41"/>
       <c r="B12" s="95"/>
       <c r="C12" s="38"/>
@@ -7539,7 +7574,7 @@
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
     </row>
-    <row r="13" spans="1:9" s="40" customFormat="1" ht="18">
+    <row r="13" spans="1:9" s="40" customFormat="1" ht="18.75">
       <c r="A13" s="37"/>
       <c r="B13" s="65"/>
       <c r="C13" s="38"/>
@@ -7550,7 +7585,7 @@
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
     </row>
-    <row r="14" spans="1:9" s="40" customFormat="1" ht="18">
+    <row r="14" spans="1:9" s="40" customFormat="1" ht="18.75">
       <c r="A14" s="41"/>
       <c r="B14" s="60"/>
       <c r="C14" s="57"/>
@@ -7561,7 +7596,7 @@
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
     </row>
-    <row r="15" spans="1:9" s="40" customFormat="1" ht="18">
+    <row r="15" spans="1:9" s="40" customFormat="1" ht="18.75">
       <c r="A15" s="41"/>
       <c r="B15" s="60"/>
       <c r="C15" s="57"/>
@@ -7572,7 +7607,7 @@
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
     </row>
-    <row r="16" spans="1:9" s="40" customFormat="1" ht="18">
+    <row r="16" spans="1:9" s="40" customFormat="1" ht="18.75">
       <c r="A16" s="41"/>
       <c r="B16" s="60"/>
       <c r="C16" s="57"/>
@@ -7583,7 +7618,7 @@
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
     </row>
-    <row r="17" spans="1:9" s="40" customFormat="1" ht="18.600000000000001" thickBot="1">
+    <row r="17" spans="1:9" s="40" customFormat="1" ht="19.5" thickBot="1">
       <c r="A17" s="44"/>
       <c r="B17" s="61"/>
       <c r="C17" s="43"/>
@@ -7594,13 +7629,13 @@
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
     </row>
-    <row r="18" spans="1:9" s="40" customFormat="1" ht="18.600000000000001" thickBot="1">
-      <c r="A18" s="216" t="s">
+    <row r="18" spans="1:9" s="40" customFormat="1" ht="19.5" thickBot="1">
+      <c r="A18" s="219" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="217"/>
-      <c r="C18" s="217"/>
-      <c r="D18" s="218"/>
+      <c r="B18" s="220"/>
+      <c r="C18" s="220"/>
+      <c r="D18" s="221"/>
       <c r="E18" s="56">
         <f>SUM(E3:E17)</f>
         <v>0</v>
@@ -7613,28 +7648,28 @@
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
     </row>
-    <row r="19" spans="1:9" ht="14.4" thickBot="1">
-      <c r="A19" s="221" t="s">
+    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A19" s="224" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="222"/>
-      <c r="C19" s="222"/>
-      <c r="D19" s="222"/>
-      <c r="E19" s="222"/>
-      <c r="F19" s="223"/>
+      <c r="B19" s="225"/>
+      <c r="C19" s="225"/>
+      <c r="D19" s="225"/>
+      <c r="E19" s="225"/>
+      <c r="F19" s="226"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="18" thickBot="1">
-      <c r="A20" s="212" t="s">
+    <row r="20" spans="1:9" ht="19.5" thickBot="1">
+      <c r="A20" s="215" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="212"/>
-      <c r="C20" s="212"/>
-      <c r="D20" s="212"/>
-    </row>
-    <row r="21" spans="1:9" ht="78.599999999999994" thickBot="1">
+      <c r="B20" s="215"/>
+      <c r="C20" s="215"/>
+      <c r="D20" s="215"/>
+    </row>
+    <row r="21" spans="1:9" ht="79.5" thickBot="1">
       <c r="A21" s="47" t="s">
         <v>44</v>
       </c>
@@ -7654,7 +7689,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="18">
+    <row r="22" spans="1:9" ht="18.75">
       <c r="A22" s="90"/>
       <c r="B22" s="84"/>
       <c r="C22" s="71"/>
@@ -7662,7 +7697,7 @@
       <c r="E22" s="90"/>
       <c r="F22" s="73"/>
     </row>
-    <row r="23" spans="1:9" ht="18">
+    <row r="23" spans="1:9" ht="18.75">
       <c r="A23" s="91"/>
       <c r="B23" s="85"/>
       <c r="C23" s="75"/>
@@ -7670,7 +7705,7 @@
       <c r="E23" s="98"/>
       <c r="F23" s="75"/>
     </row>
-    <row r="24" spans="1:9" ht="18">
+    <row r="24" spans="1:9" ht="18.75">
       <c r="A24" s="91"/>
       <c r="B24" s="86"/>
       <c r="C24" s="76"/>
@@ -7678,7 +7713,7 @@
       <c r="E24" s="99"/>
       <c r="F24" s="77"/>
     </row>
-    <row r="25" spans="1:9" ht="15.6">
+    <row r="25" spans="1:9" ht="15.75">
       <c r="A25" s="75"/>
       <c r="B25" s="78"/>
       <c r="C25" s="74"/>
@@ -7686,7 +7721,7 @@
       <c r="E25" s="74"/>
       <c r="F25" s="75"/>
     </row>
-    <row r="26" spans="1:9" ht="15.6">
+    <row r="26" spans="1:9" ht="15.75">
       <c r="A26" s="74"/>
       <c r="B26" s="79"/>
       <c r="C26" s="75"/>
@@ -7694,7 +7729,7 @@
       <c r="E26" s="75"/>
       <c r="F26" s="75"/>
     </row>
-    <row r="27" spans="1:9" ht="18">
+    <row r="27" spans="1:9" ht="18.75">
       <c r="A27" s="41"/>
       <c r="B27" s="80"/>
       <c r="C27" s="41"/>
@@ -7702,7 +7737,7 @@
       <c r="E27" s="41"/>
       <c r="F27" s="41"/>
     </row>
-    <row r="28" spans="1:9" ht="18">
+    <row r="28" spans="1:9" ht="18.75">
       <c r="A28" s="41"/>
       <c r="B28" s="81"/>
       <c r="C28" s="41"/>
@@ -7710,7 +7745,7 @@
       <c r="E28" s="41"/>
       <c r="F28" s="41"/>
     </row>
-    <row r="29" spans="1:9" ht="18.600000000000001" thickBot="1">
+    <row r="29" spans="1:9" ht="19.5" thickBot="1">
       <c r="A29" s="50"/>
       <c r="B29" s="81"/>
       <c r="C29" s="50"/>
@@ -7718,13 +7753,13 @@
       <c r="E29" s="50"/>
       <c r="F29" s="50"/>
     </row>
-    <row r="30" spans="1:9" ht="18.600000000000001" thickBot="1">
-      <c r="A30" s="216" t="s">
+    <row r="30" spans="1:9" ht="19.5" thickBot="1">
+      <c r="A30" s="219" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="217"/>
-      <c r="C30" s="217"/>
-      <c r="D30" s="219"/>
+      <c r="B30" s="220"/>
+      <c r="C30" s="220"/>
+      <c r="D30" s="222"/>
       <c r="E30" s="56">
         <f>SUM(E22:E29)</f>
         <v>0</v>
@@ -7734,26 +7769,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="14.4" thickBot="1">
-      <c r="A31" s="213" t="str">
+    <row r="31" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A31" s="216" t="str">
         <f>A19</f>
         <v>Викладач ______________      Завідувач кафедри  ____________       / Ігор ГАМАЮН /</v>
       </c>
-      <c r="B31" s="214"/>
-      <c r="C31" s="214"/>
-      <c r="D31" s="214"/>
-      <c r="E31" s="214"/>
-      <c r="F31" s="215"/>
-    </row>
-    <row r="32" spans="1:9" ht="18" thickBot="1">
-      <c r="A32" s="212" t="s">
+      <c r="B31" s="217"/>
+      <c r="C31" s="217"/>
+      <c r="D31" s="217"/>
+      <c r="E31" s="217"/>
+      <c r="F31" s="218"/>
+    </row>
+    <row r="32" spans="1:9" ht="19.5" thickBot="1">
+      <c r="A32" s="215" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="212"/>
-      <c r="C32" s="212"/>
-      <c r="D32" s="212"/>
-    </row>
-    <row r="33" spans="1:6" ht="47.4" thickBot="1">
+      <c r="B32" s="215"/>
+      <c r="C32" s="215"/>
+      <c r="D32" s="215"/>
+    </row>
+    <row r="33" spans="1:6" ht="48" thickBot="1">
       <c r="A33" s="51" t="s">
         <v>44</v>
       </c>
@@ -7773,7 +7808,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18.600000000000001" thickBot="1">
+    <row r="34" spans="1:6" ht="19.5" thickBot="1">
       <c r="A34" s="88"/>
       <c r="B34" s="87"/>
       <c r="C34" s="63"/>
@@ -7781,7 +7816,7 @@
       <c r="E34" s="92"/>
       <c r="F34" s="63"/>
     </row>
-    <row r="35" spans="1:6" ht="18">
+    <row r="35" spans="1:6" ht="18.75">
       <c r="A35" s="89"/>
       <c r="B35" s="87"/>
       <c r="C35" s="35"/>
@@ -7789,7 +7824,7 @@
       <c r="E35" s="41"/>
       <c r="F35" s="37"/>
     </row>
-    <row r="36" spans="1:6" ht="15.6">
+    <row r="36" spans="1:6" ht="15.75">
       <c r="A36" s="35"/>
       <c r="B36" s="82"/>
       <c r="C36" s="35"/>
@@ -7797,7 +7832,7 @@
       <c r="E36" s="37"/>
       <c r="F36" s="37"/>
     </row>
-    <row r="37" spans="1:6" ht="18">
+    <row r="37" spans="1:6" ht="18.75">
       <c r="A37" s="41"/>
       <c r="B37" s="83"/>
       <c r="C37" s="41"/>
@@ -7805,7 +7840,7 @@
       <c r="E37" s="41"/>
       <c r="F37" s="41"/>
     </row>
-    <row r="38" spans="1:6" ht="18.600000000000001" thickBot="1">
+    <row r="38" spans="1:6" ht="19.5" thickBot="1">
       <c r="A38" s="41"/>
       <c r="B38" s="83"/>
       <c r="C38" s="41"/>
@@ -7813,13 +7848,13 @@
       <c r="E38" s="41"/>
       <c r="F38" s="41"/>
     </row>
-    <row r="39" spans="1:6" s="40" customFormat="1" ht="18.600000000000001" thickBot="1">
-      <c r="A39" s="220" t="s">
+    <row r="39" spans="1:6" s="40" customFormat="1" ht="19.5" thickBot="1">
+      <c r="A39" s="223" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="217"/>
-      <c r="C39" s="217"/>
-      <c r="D39" s="219"/>
+      <c r="B39" s="220"/>
+      <c r="C39" s="220"/>
+      <c r="D39" s="222"/>
       <c r="E39" s="56">
         <f>SUM(E34:E38)</f>
         <v>0</v>
@@ -7829,16 +7864,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="14.4" thickBot="1">
-      <c r="A40" s="213" t="str">
+    <row r="40" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A40" s="216" t="str">
         <f>A31</f>
         <v>Викладач ______________      Завідувач кафедри  ____________       / Ігор ГАМАЮН /</v>
       </c>
-      <c r="B40" s="214"/>
-      <c r="C40" s="214"/>
-      <c r="D40" s="214"/>
-      <c r="E40" s="214"/>
-      <c r="F40" s="215"/>
+      <c r="B40" s="217"/>
+      <c r="C40" s="217"/>
+      <c r="D40" s="217"/>
+      <c r="E40" s="217"/>
+      <c r="F40" s="218"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1"/>
@@ -7870,34 +7905,34 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" style="125" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="125" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" style="125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="125" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="125" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="125" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="125"/>
+    <col min="1" max="1" width="5.42578125" style="125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="125" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" style="125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="125" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="227" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
     </row>
     <row r="2" spans="1:7" ht="50.25" customHeight="1" thickBot="1">
       <c r="A2" s="138" t="s">
@@ -7987,184 +8022,179 @@
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1"/>
     <row r="11" spans="1:7" ht="18" customHeight="1" thickBot="1">
-      <c r="A11" s="232" t="s">
+      <c r="A11" s="227" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="232"/>
-      <c r="C11" s="232"/>
-      <c r="D11" s="232"/>
-      <c r="E11" s="232"/>
-      <c r="F11" s="232"/>
-      <c r="G11" s="232"/>
+      <c r="B11" s="227"/>
+      <c r="C11" s="227"/>
+      <c r="D11" s="227"/>
+      <c r="E11" s="227"/>
+      <c r="F11" s="227"/>
+      <c r="G11" s="227"/>
     </row>
     <row r="12" spans="1:7" ht="52.5" customHeight="1" thickBot="1">
       <c r="A12" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="235" t="s">
+      <c r="B12" s="228" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="235"/>
-      <c r="D12" s="235"/>
-      <c r="E12" s="235"/>
-      <c r="F12" s="235"/>
+      <c r="C12" s="228"/>
+      <c r="D12" s="228"/>
+      <c r="E12" s="228"/>
+      <c r="F12" s="228"/>
       <c r="G12" s="150" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="52.5" customHeight="1">
       <c r="A13" s="147"/>
-      <c r="B13" s="236"/>
-      <c r="C13" s="237"/>
-      <c r="D13" s="237"/>
-      <c r="E13" s="237"/>
-      <c r="F13" s="238"/>
+      <c r="B13" s="229"/>
+      <c r="C13" s="230"/>
+      <c r="D13" s="230"/>
+      <c r="E13" s="230"/>
+      <c r="F13" s="231"/>
       <c r="G13" s="148"/>
     </row>
     <row r="14" spans="1:7" ht="42.75" customHeight="1">
       <c r="A14" s="132"/>
-      <c r="B14" s="239" t="s">
+      <c r="B14" s="232" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="240"/>
-      <c r="D14" s="240"/>
-      <c r="E14" s="240"/>
-      <c r="F14" s="241"/>
+      <c r="C14" s="233"/>
+      <c r="D14" s="233"/>
+      <c r="E14" s="233"/>
+      <c r="F14" s="234"/>
       <c r="G14" s="131"/>
     </row>
     <row r="15" spans="1:7" ht="33.75" customHeight="1">
       <c r="A15" s="132"/>
-      <c r="B15" s="226"/>
-      <c r="C15" s="227"/>
-      <c r="D15" s="227"/>
-      <c r="E15" s="227"/>
-      <c r="F15" s="228"/>
+      <c r="B15" s="237"/>
+      <c r="C15" s="238"/>
+      <c r="D15" s="238"/>
+      <c r="E15" s="238"/>
+      <c r="F15" s="239"/>
       <c r="G15" s="131"/>
     </row>
     <row r="16" spans="1:7" ht="31.5" customHeight="1">
       <c r="A16" s="132"/>
-      <c r="B16" s="226"/>
-      <c r="C16" s="227"/>
-      <c r="D16" s="227"/>
-      <c r="E16" s="227"/>
-      <c r="F16" s="228"/>
+      <c r="B16" s="237"/>
+      <c r="C16" s="238"/>
+      <c r="D16" s="238"/>
+      <c r="E16" s="238"/>
+      <c r="F16" s="239"/>
       <c r="G16" s="131"/>
     </row>
     <row r="17" spans="1:7" ht="32.25" customHeight="1">
       <c r="A17" s="132"/>
-      <c r="B17" s="226"/>
-      <c r="C17" s="227"/>
-      <c r="D17" s="227"/>
-      <c r="E17" s="227"/>
-      <c r="F17" s="228"/>
+      <c r="B17" s="237"/>
+      <c r="C17" s="238"/>
+      <c r="D17" s="238"/>
+      <c r="E17" s="238"/>
+      <c r="F17" s="239"/>
       <c r="G17" s="131"/>
     </row>
     <row r="18" spans="1:7" ht="31.5" customHeight="1" thickBot="1">
       <c r="A18" s="130"/>
-      <c r="B18" s="229"/>
-      <c r="C18" s="230"/>
-      <c r="D18" s="230"/>
-      <c r="E18" s="230"/>
-      <c r="F18" s="231"/>
+      <c r="B18" s="240"/>
+      <c r="C18" s="241"/>
+      <c r="D18" s="241"/>
+      <c r="E18" s="241"/>
+      <c r="F18" s="242"/>
       <c r="G18" s="129"/>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:7" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A20" s="232" t="s">
+      <c r="A20" s="227" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="232"/>
-      <c r="C20" s="232"/>
-      <c r="D20" s="232"/>
-      <c r="E20" s="232"/>
-      <c r="F20" s="232"/>
-      <c r="G20" s="232"/>
+      <c r="B20" s="227"/>
+      <c r="C20" s="227"/>
+      <c r="D20" s="227"/>
+      <c r="E20" s="227"/>
+      <c r="F20" s="227"/>
+      <c r="G20" s="227"/>
     </row>
     <row r="21" spans="1:7" ht="30.75" customHeight="1" thickBot="1">
       <c r="A21" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="233" t="s">
+      <c r="B21" s="243" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="233"/>
-      <c r="D21" s="233"/>
-      <c r="E21" s="233"/>
-      <c r="F21" s="233"/>
+      <c r="C21" s="243"/>
+      <c r="D21" s="243"/>
+      <c r="E21" s="243"/>
+      <c r="F21" s="243"/>
       <c r="G21" s="135" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30.75" customHeight="1">
       <c r="A22" s="134"/>
-      <c r="B22" s="234"/>
-      <c r="C22" s="234"/>
-      <c r="D22" s="234"/>
-      <c r="E22" s="234"/>
-      <c r="F22" s="234"/>
+      <c r="B22" s="244"/>
+      <c r="C22" s="244"/>
+      <c r="D22" s="244"/>
+      <c r="E22" s="244"/>
+      <c r="F22" s="244"/>
       <c r="G22" s="133"/>
     </row>
     <row r="23" spans="1:7" ht="34.5" customHeight="1">
       <c r="A23" s="132"/>
-      <c r="B23" s="224"/>
-      <c r="C23" s="224"/>
-      <c r="D23" s="224"/>
-      <c r="E23" s="224"/>
-      <c r="F23" s="224"/>
+      <c r="B23" s="235"/>
+      <c r="C23" s="235"/>
+      <c r="D23" s="235"/>
+      <c r="E23" s="235"/>
+      <c r="F23" s="235"/>
       <c r="G23" s="131"/>
     </row>
     <row r="24" spans="1:7" ht="30.75" customHeight="1">
       <c r="A24" s="132"/>
-      <c r="B24" s="224"/>
-      <c r="C24" s="224"/>
-      <c r="D24" s="224"/>
-      <c r="E24" s="224"/>
-      <c r="F24" s="224"/>
+      <c r="B24" s="235"/>
+      <c r="C24" s="235"/>
+      <c r="D24" s="235"/>
+      <c r="E24" s="235"/>
+      <c r="F24" s="235"/>
       <c r="G24" s="131"/>
     </row>
     <row r="25" spans="1:7" ht="33.75" customHeight="1">
       <c r="A25" s="132"/>
-      <c r="B25" s="224"/>
-      <c r="C25" s="224"/>
-      <c r="D25" s="224"/>
-      <c r="E25" s="224"/>
-      <c r="F25" s="224"/>
+      <c r="B25" s="235"/>
+      <c r="C25" s="235"/>
+      <c r="D25" s="235"/>
+      <c r="E25" s="235"/>
+      <c r="F25" s="235"/>
       <c r="G25" s="131"/>
     </row>
     <row r="26" spans="1:7" ht="30.75" customHeight="1">
       <c r="A26" s="132"/>
-      <c r="B26" s="224"/>
-      <c r="C26" s="224"/>
-      <c r="D26" s="224"/>
-      <c r="E26" s="224"/>
-      <c r="F26" s="224"/>
+      <c r="B26" s="235"/>
+      <c r="C26" s="235"/>
+      <c r="D26" s="235"/>
+      <c r="E26" s="235"/>
+      <c r="F26" s="235"/>
       <c r="G26" s="131"/>
     </row>
     <row r="27" spans="1:7" ht="33" customHeight="1">
       <c r="A27" s="132"/>
-      <c r="B27" s="224"/>
-      <c r="C27" s="224"/>
-      <c r="D27" s="224"/>
-      <c r="E27" s="224"/>
-      <c r="F27" s="224"/>
+      <c r="B27" s="235"/>
+      <c r="C27" s="235"/>
+      <c r="D27" s="235"/>
+      <c r="E27" s="235"/>
+      <c r="F27" s="235"/>
       <c r="G27" s="131"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" customHeight="1" thickBot="1">
       <c r="A28" s="130"/>
-      <c r="B28" s="225"/>
-      <c r="C28" s="225"/>
-      <c r="D28" s="225"/>
-      <c r="E28" s="225"/>
-      <c r="F28" s="225"/>
+      <c r="B28" s="236"/>
+      <c r="C28" s="236"/>
+      <c r="D28" s="236"/>
+      <c r="E28" s="236"/>
+      <c r="F28" s="236"/>
       <c r="G28" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="B15:F15"/>
@@ -8178,6 +8208,11 @@
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B25:F25"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="81" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>